<commit_message>
creacion de la funcion consultar persona
</commit_message>
<xml_diff>
--- a/BaseCrudColabPersona.xlsx
+++ b/BaseCrudColabPersona.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\repo\gitflow_practica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F459258B-6B47-4643-8EAA-7BC2C591FD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F026B26-02F0-434F-8F2D-03BCB1D0DEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="persona" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">id </t>
   </si>
@@ -43,16 +43,54 @@
   </si>
   <si>
     <t>nacimiento</t>
+  </si>
+  <si>
+    <t>frank</t>
+  </si>
+  <si>
+    <t>fra@gmail.com</t>
+  </si>
+  <si>
+    <t>daniel</t>
+  </si>
+  <si>
+    <t>yoyo</t>
+  </si>
+  <si>
+    <t>perez</t>
+  </si>
+  <si>
+    <t>albeiro</t>
+  </si>
+  <si>
+    <t>fweq@gmail.com</t>
+  </si>
+  <si>
+    <t>asdas@gmail.com</t>
+  </si>
+  <si>
+    <t>asdfsf@gmail.com</t>
+  </si>
+  <si>
+    <t>dadas@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +113,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -360,18 +402,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -395,7 +437,114 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>123456</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>123456</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2">
+        <v>39084</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>123456</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2">
+        <v>39450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>123456</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2">
+        <v>39817</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>123456</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2">
+        <v>40183</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{3175295A-8BAA-4889-8E0B-AE2142553891}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{E596A373-E1DE-4891-B9BB-596DB5854349}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{EEA7C7B3-7086-47C8-8D21-C962EC6F902D}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{A9E56A73-7A9A-4B3F-BD0C-D0A5D6EBF2E9}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{EC8203C4-CA3D-473E-BF46-8A6E35CACC44}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
creando funcion de actualizar persona
</commit_message>
<xml_diff>
--- a/BaseCrudColabPersona.xlsx
+++ b/BaseCrudColabPersona.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\repo\gitflow_practica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F459258B-6B47-4643-8EAA-7BC2C591FD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1D6D9E-CD26-4117-A91C-3D24B7C50EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="persona" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">id </t>
   </si>
@@ -43,16 +38,33 @@
   </si>
   <si>
     <t>nacimiento</t>
+  </si>
+  <si>
+    <t>frank</t>
+  </si>
+  <si>
+    <t>frankrcuetia@gmail.com</t>
+  </si>
+  <si>
+    <t>24/02/2005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +87,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -360,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,7 +411,31 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>157799</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
creando la funcion de agregar persona
</commit_message>
<xml_diff>
--- a/BaseCrudColabPersona.xlsx
+++ b/BaseCrudColabPersona.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\repo\gitflow_practica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634D7E25-7B89-409D-9F76-BF2AF21D92C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0C48CE-EA0A-4AE2-8EF9-F63D5EB1BF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="persona" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">id </t>
   </si>
@@ -48,19 +43,28 @@
     <t>frank</t>
   </si>
   <si>
+    <t>frank@gmail.com</t>
+  </si>
+  <si>
     <t>yoiner</t>
   </si>
   <si>
+    <t>yoiner@gmail.com</t>
+  </si>
+  <si>
     <t>juancho</t>
   </si>
   <si>
-    <t>frank@gmail.com</t>
-  </si>
-  <si>
-    <t>yoiner@gmail.com</t>
-  </si>
-  <si>
     <t>gay@gmail.com</t>
+  </si>
+  <si>
+    <t>alex</t>
+  </si>
+  <si>
+    <t>alex@gmail.com</t>
+  </si>
+  <si>
+    <t>01/12/2005</t>
   </si>
 </sst>
 </file>
@@ -103,7 +107,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -390,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +443,7 @@
         <v>57348953</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2">
         <v>38407</v>
@@ -450,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>19</v>
@@ -459,7 +463,7 @@
         <v>45378</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2">
         <v>37881</v>
@@ -470,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -483,13 +487,33 @@
       </c>
       <c r="F4" s="2">
         <v>44794</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>9789485</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{065D1FF8-683A-4AED-9511-3BADC0879B01}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{4F16F418-3CAB-4D62-B00D-5E0D06BBFE2D}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{EE15B597-2CDC-43FF-8CED-9549042130EB}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
creando la funcion de eliminar persona
</commit_message>
<xml_diff>
--- a/BaseCrudColabPersona.xlsx
+++ b/BaseCrudColabPersona.xlsx
@@ -1,92 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\repo\gitflow_practica\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634D7E25-7B89-409D-9F76-BF2AF21D92C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="persona" sheetId="1" r:id="rId1"/>
+    <sheet name="persona" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">id </t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>edad</t>
-  </si>
-  <si>
-    <t>telefono</t>
-  </si>
-  <si>
-    <t>correo</t>
-  </si>
-  <si>
-    <t>nacimiento</t>
-  </si>
-  <si>
-    <t>frank</t>
-  </si>
-  <si>
-    <t>yoiner</t>
-  </si>
-  <si>
-    <t>juancho</t>
-  </si>
-  <si>
-    <t>frank@gmail.com</t>
-  </si>
-  <si>
-    <t>yoiner@gmail.com</t>
-  </si>
-  <si>
-    <t>gay@gmail.com</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -103,27 +52,86 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -389,107 +397,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col width="2.85546875" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="5.28515625" customWidth="1" min="3" max="3"/>
+    <col width="6.42578125" customWidth="1" min="5" max="5"/>
+    <col width="11.140625" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">id </t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>edad</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>telefono</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>correo</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>nacimiento</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frank</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" t="n">
+        <v>57348953</v>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>frank@gmail.com</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>38407</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" s="1" t="inlineStr"/>
+      <c r="F3" s="2" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>57348953</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2">
-        <v>38407</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>19</v>
-      </c>
-      <c r="D3">
-        <v>45378</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2">
-        <v>37881</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>juancho</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>18</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>7485378</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>gay@gmail.com</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n">
         <v>44794</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{065D1FF8-683A-4AED-9511-3BADC0879B01}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{4F16F418-3CAB-4D62-B00D-5E0D06BBFE2D}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{EE15B597-2CDC-43FF-8CED-9549042130EB}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
funciones de persona terminado
</commit_message>
<xml_diff>
--- a/BaseCrudColabPersona.xlsx
+++ b/BaseCrudColabPersona.xlsx
@@ -1,96 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\repo\gitflow_practica\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0C48CE-EA0A-4AE2-8EF9-F63D5EB1BF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="persona" sheetId="1" r:id="rId1"/>
+    <sheet name="persona" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">id </t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>edad</t>
-  </si>
-  <si>
-    <t>telefono</t>
-  </si>
-  <si>
-    <t>correo</t>
-  </si>
-  <si>
-    <t>nacimiento</t>
-  </si>
-  <si>
-    <t>frank</t>
-  </si>
-  <si>
-    <t>frank@gmail.com</t>
-  </si>
-  <si>
-    <t>yoiner</t>
-  </si>
-  <si>
-    <t>yoiner@gmail.com</t>
-  </si>
-  <si>
-    <t>juancho</t>
-  </si>
-  <si>
-    <t>gay@gmail.com</t>
-  </si>
-  <si>
-    <t>alex</t>
-  </si>
-  <si>
-    <t>alex@gmail.com</t>
-  </si>
-  <si>
-    <t>01/12/2005</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -110,24 +55,83 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -393,127 +397,179 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col width="2.85546875" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="5.28515625" customWidth="1" min="3" max="3"/>
+    <col width="6.42578125" customWidth="1" min="5" max="5"/>
+    <col width="11.140625" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">id </t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>edad</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>telefono</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>correo</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>nacimiento</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frank</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" t="n">
+        <v>57348953</v>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>frank@gmail.com</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>38407</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>yoiner</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>19</v>
+      </c>
+      <c r="D3" t="n">
+        <v>45378</v>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>yoiner@gmail.com</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>37881</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>daniel</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>111111111</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>daniel@gmila.com</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>17/02/2003</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>57348953</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2">
-        <v>38407</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>19</v>
-      </c>
-      <c r="D3">
-        <v>45378</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2">
-        <v>37881</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>7485378</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2">
-        <v>44794</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>9789485</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>breynner</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2222222</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>b@gmail.com</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>14/25/2023</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>